<commit_message>
20230503 - updated summaries
</commit_message>
<xml_diff>
--- a/summary/20230502_certificates_MPS.xlsx
+++ b/summary/20230502_certificates_MPS.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="20230502-Certificates" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t xml:space="preserve">Google data analytics professional certificate</t>
   </si>
@@ -113,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">Structuring Machine Learning Projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convolutional Neural Networks</t>
   </si>
   <si>
     <t xml:space="preserve">Extra </t>
@@ -275,6 +279,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -296,18 +301,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF161616"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -379,80 +387,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -533,555 +537,435 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:F50"/>
+  <dimension ref="B3:F51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F53" activeCellId="0" sqref="F53"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="75.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="56.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="75.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="56.8"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="5"/>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="5"/>
-      <c r="C29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="8" t="s">
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="6"/>
+      <c r="C30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="5"/>
-      <c r="C30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>36</v>
-      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="12"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="6"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="F34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="5"/>
-      <c r="C35" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="14" t="n">
-        <v>0.9658</v>
-      </c>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="F35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="5"/>
-      <c r="C36" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="14" t="n">
-        <v>1</v>
-      </c>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="5"/>
-      <c r="C37" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="14" t="n">
-        <v>1</v>
-      </c>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="5"/>
-      <c r="C38" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="14" t="n">
-        <v>0.8851</v>
-      </c>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="5"/>
-      <c r="C39" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" s="14" t="n">
-        <v>0.9286</v>
-      </c>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="F39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="5"/>
-      <c r="C40" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="14" t="n">
-        <v>0.9686</v>
-      </c>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="F40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="5"/>
-      <c r="C41" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F41" s="14" t="n">
-        <v>0.8919</v>
-      </c>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="5"/>
-      <c r="C42" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" s="14" t="n">
-        <v>0.878</v>
-      </c>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="5"/>
-      <c r="C43" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F43" s="14" t="n">
-        <v>1</v>
-      </c>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="5"/>
-      <c r="C44" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F44" s="14" t="n">
-        <v>0.9894</v>
-      </c>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="5"/>
-      <c r="C45" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F45" s="14" t="n">
-        <v>0.9268</v>
-      </c>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+      <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="5"/>
-      <c r="C46" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" s="14" t="n">
-        <v>1</v>
-      </c>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+      <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="5"/>
-      <c r="C47" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F47" s="14" t="n">
-        <v>0.9556</v>
-      </c>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+      <c r="F47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="5"/>
-      <c r="C48" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F48" s="14" t="n">
-        <v>1</v>
-      </c>
+      <c r="B48" s="0"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+      <c r="F48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="5"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="B49" s="0"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="F49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="5"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="E50" s="16"/>
-      <c r="F50" s="17" t="n">
-        <f aca="false">AVERAGE(F35:F48)</f>
-        <v>0.956414285714286</v>
-      </c>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="F50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+      <c r="F51" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B33:D33"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.954166666666667" bottom="0.7875" header="0.7875" footer="0.511811023622047"/>
@@ -1091,4 +975,283 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:F19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.32"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="13"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="15" t="n">
+        <v>0.9658</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="15" t="n">
+        <v>0.8851</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="15" t="n">
+        <v>0.9286</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="15" t="n">
+        <v>0.9686</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="15" t="n">
+        <v>0.8919</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="15" t="n">
+        <v>0.878</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="15" t="n">
+        <v>0.9894</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="15" t="n">
+        <v>0.9268</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="15" t="n">
+        <v>0.9556</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17" t="n">
+        <f aca="false">AVERAGE(F4:F17)</f>
+        <v>0.956414285714286</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>